<commit_message>
add new toy version
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/stimuli_MultiplEYE_toy_x_x_1_1/multipleye_comprehension_questions_toy.xlsx
+++ b/experiment_implementation/data/stimuli_MultiplEYE_toy_x_x_1_1/multipleye_comprehension_questions_toy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_MultiplEYE_toy_x_x_1_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation-2/data/stimuli_MultiplEYE_toy_x_x_1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CD4593-ECEB-324A-9B27-9FA9E722A2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E28C92-D11C-4746-A6E1-CF185D33F7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_comprehension_questi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -180,19 +180,22 @@
     <t>George Eliot - Middlemarch</t>
   </si>
   <si>
-    <t>Emily Bront√´ - Wuthering heights</t>
-  </si>
-  <si>
-    <t>Mary Shelley - Frankenstein¬†</t>
-  </si>
-  <si>
     <t>Jane Austen - Pride and Prejudice</t>
+  </si>
+  <si>
+    <t>Emily Bront - Wuthering heights</t>
+  </si>
+  <si>
+    <t>Mary Shelley - Frankenstein</t>
+  </si>
+  <si>
+    <t>stimulus_text_without_annotated_spans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1049,16 +1052,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1081,43 +1084,46 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1139,44 +1145,47 @@
       <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>32</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1198,38 +1207,41 @@
       <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1251,38 +1263,41 @@
       <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>38</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>33</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>32</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1305,16 +1320,16 @@
         <v>48</v>
       </c>
       <c r="H5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>50</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
       </c>
       <c r="L5" t="s">
         <v>52</v>
@@ -1322,16 +1337,19 @@
       <c r="M5" t="s">
         <v>53</v>
       </c>
-      <c r="P5" t="s">
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>31</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>32</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
toy data with newly added screens
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/stimuli_MultiplEYE_toy_x_x_1_1/multipleye_comprehension_questions_toy.xlsx
+++ b/experiment_implementation/data/stimuli_MultiplEYE_toy_x_x_1_1/multipleye_comprehension_questions_toy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation-2/data/stimuli_MultiplEYE_toy_x_x_1_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_MultiplEYE_toy_x_x_1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E28C92-D11C-4746-A6E1-CF185D33F7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CD4593-ECEB-324A-9B27-9FA9E722A2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_comprehension_questi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -180,22 +180,19 @@
     <t>George Eliot - Middlemarch</t>
   </si>
   <si>
+    <t>Emily Bront√´ - Wuthering heights</t>
+  </si>
+  <si>
+    <t>Mary Shelley - Frankenstein¬†</t>
+  </si>
+  <si>
     <t>Jane Austen - Pride and Prejudice</t>
-  </si>
-  <si>
-    <t>Emily Bront - Wuthering heights</t>
-  </si>
-  <si>
-    <t>Mary Shelley - Frankenstein</t>
-  </si>
-  <si>
-    <t>stimulus_text_without_annotated_spans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1052,16 +1049,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,46 +1081,43 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1145,47 +1139,44 @@
       <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1207,41 +1198,38 @@
       <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>35</v>
+      <c r="H3" t="s">
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" t="s">
         <v>40</v>
       </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1263,41 +1251,38 @@
       <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>41</v>
+      <c r="H4" t="s">
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" t="s">
         <v>38</v>
       </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1320,16 +1305,16 @@
         <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
         <v>52</v>
@@ -1337,19 +1322,16 @@
       <c r="M5" t="s">
         <v>53</v>
       </c>
-      <c r="N5" t="s">
-        <v>51</v>
+      <c r="P5" t="s">
+        <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>